<commit_message>
adds more companies to the dataset
</commit_message>
<xml_diff>
--- a/data/SOFT-3.xlsx
+++ b/data/SOFT-3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdi/Documents/Teaching/DS/2023/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Google Drive\Computer Science\SOFT\Semester 1\Data science\Assignments\internship data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90420F14-0C7F-5845-AAFC-8DFB1B29B5D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B90142-713C-42B0-84D2-198291745F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="3820" windowWidth="24000" windowHeight="12980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Benjamin Curovic</t>
   </si>
@@ -133,13 +133,52 @@
   </si>
   <si>
     <t>SOFT Internship 2023</t>
+  </si>
+  <si>
+    <t>Wash World</t>
+  </si>
+  <si>
+    <t>Carve</t>
+  </si>
+  <si>
+    <t>GroupM</t>
+  </si>
+  <si>
+    <t>Brøndbyernes I.F.</t>
+  </si>
+  <si>
+    <t>Meew</t>
+  </si>
+  <si>
+    <t>Funelo</t>
+  </si>
+  <si>
+    <t>PreCure</t>
+  </si>
+  <si>
+    <t>Wilke</t>
+  </si>
+  <si>
+    <t>OOONO</t>
+  </si>
+  <si>
+    <t>Elbek &amp; Vejrup</t>
+  </si>
+  <si>
+    <t>Ellab</t>
+  </si>
+  <si>
+    <t>Lejka</t>
+  </si>
+  <si>
+    <t>Firi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +206,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -176,7 +221,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -199,15 +244,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,24 +547,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8E2F56-462D-A74B-8557-45B0A89EEC31}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
@@ -513,7 +572,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -529,7 +588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -537,7 +596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -545,7 +604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -553,7 +612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
@@ -561,7 +620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -569,7 +628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -577,7 +636,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
@@ -585,7 +644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
@@ -593,7 +652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
@@ -601,7 +660,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
@@ -609,7 +668,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
@@ -617,7 +676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
@@ -625,7 +684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
@@ -633,7 +692,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
@@ -641,7 +700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
@@ -649,7 +708,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
@@ -657,12 +716,77 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -670,19 +794,11 @@
     <dataValidation showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Opslag (påkrævet)" prompt="Denne post af typen Studerende skal allerede findes i Microsoft Dynamics 365 eller i denne kildefil." sqref="B3:B21" xr:uid="{84F23E93-6B6B-8641-8A27-A6CC2CFC9F66}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050E7AEDA699A6046B28BDB03A4B3ACE5" ma:contentTypeVersion="30" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c60638a9c0b28c271ac4d4f2b9c4b86e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7d4bd1a6-963b-4ce5-9d6a-82f9bec88dc5" xmlns:ns3="d40e101a-1fec-4fbd-a9d0-ed41492f4cd8" xmlns:ns4="c3c11eb6-de36-4131-bab2-6a22847efc48" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c3069844a3c7ac327c702fd6e0bb596b" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -977,6 +1093,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1006,14 +1131,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45D47333-C5EE-4748-B295-5B02675A6229}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD114C5A-7016-4515-BAAA-FCC1ACD965C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1034,6 +1151,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45D47333-C5EE-4748-B295-5B02675A6229}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17B4FFF1-E645-40CC-91A8-95B75F9C57B2}">
   <ds:schemaRefs>

</xml_diff>